<commit_message>
Working on comp 240 Flask
</commit_message>
<xml_diff>
--- a/Python/Comp 230/invoice.xlsx
+++ b/Python/Comp 230/invoice.xlsx
@@ -3,11 +3,14 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Invoice 1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Invoice 2" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Invoice 3" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Invoice 4" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -428,7 +431,7 @@
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -549,4 +552,346 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="25" customWidth="1" min="3" max="3"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>INVOICE #2</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>customer_id</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>f_name</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>"Richmound"</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>l_name</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>"Hulmes"</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>phone</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>"941-402-4909"</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>invoice_date</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>"2020-03-07"</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>payment_method</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>"Credit"</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>total_price</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1282.5</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="25" customWidth="1" min="3" max="3"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>INVOICE #3</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>customer_id</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>f_name</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>"Annetta"</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>l_name</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>"Colleford"</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>phone</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>"198-751-6091"</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>invoice_date</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>"2020-03-08"</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>payment_method</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>"Debit"</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>total_price</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>210</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="25" customWidth="1" min="3" max="3"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>INVOICE #4</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>customer_id</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>f_name</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>"Jessalyn"</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>l_name</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>"Formie"</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>phone</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>"103-907-2970"</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>invoice_date</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>"2020-03-24"</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>payment_method</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>"Cheque"</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>total_price</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>464.5</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>